<commit_message>
Subida de vídeos en Instagram
</commit_message>
<xml_diff>
--- a/Redes Sociales/redes_sociales.xlsx
+++ b/Redes Sociales/redes_sociales.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Github\Redes_Sociales\Redes Sociales\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\noeli\Documents\GitHub\Redes_Sociales\Redes Sociales\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Youtube</t>
   </si>
@@ -105,6 +105,12 @@
   </si>
   <si>
     <t>Video de Kappa</t>
+  </si>
+  <si>
+    <t>Se ha subido algo de redes por Noelia N. Maqueda</t>
+  </si>
+  <si>
+    <t>Vídeo de Tangs, Fénix y Kappa</t>
   </si>
 </sst>
 </file>
@@ -134,7 +140,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -165,6 +171,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -178,7 +190,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -187,6 +199,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -503,11 +516,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="F68" sqref="F68"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.85546875" customWidth="1"/>
     <col min="3" max="3" width="21.140625" customWidth="1"/>
@@ -629,6 +642,10 @@
       <c r="H7" s="6" t="s">
         <v>14</v>
       </c>
+      <c r="K7" s="8"/>
+      <c r="L7" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
@@ -1301,6 +1318,9 @@
       <c r="B67" s="1">
         <v>45266</v>
       </c>
+      <c r="D67" s="8" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="68" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B68" s="1">

</xml_diff>